<commit_message>
updates on the state highway level road closure data
</commit_message>
<xml_diff>
--- a/data/derived/public/road_closures.xlsx
+++ b/data/derived/public/road_closures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsokolow\Documents\GitHub\Flooding-and-Healthcare-2024\data\derived\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A026071-872E-4B5D-8492-CDCE860EE240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B229B97A-4516-4E17-87A6-6D0EF870D50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="585" windowWidth="17085" windowHeight="15345" xr2:uid="{5778C281-5D7A-4C2F-9C6C-142270E29836}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
   <si>
     <t>Date closed</t>
   </si>
@@ -63,18 +63,6 @@
     <t>SH4</t>
   </si>
   <si>
-    <t>Detour</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>no detour</t>
-  </si>
-  <si>
-    <t>SH1 and SH49</t>
-  </si>
-  <si>
     <t>Eskdale</t>
   </si>
   <si>
@@ -105,9 +93,6 @@
     <t>Taupo</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>SH50 - SH2</t>
   </si>
   <si>
@@ -252,13 +237,16 @@
     <t>Waka Kotahi NZ Transport Agency - Hawke's Bay and Gisborne; Gisborne District Council Facebook</t>
   </si>
   <si>
-    <t>bailey bridge</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>bailey bridge replacement</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -611,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA661F5C-2962-406D-9974-AC40C62876EC}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,23 +611,22 @@
     <col min="4" max="4" width="27.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="29.140625" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -651,16 +638,13 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -668,10 +652,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1">
         <v>45334</v>
@@ -683,16 +667,13 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -700,7 +681,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -714,14 +695,14 @@
       <c r="G3">
         <v>0</v>
       </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
       <c r="I3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -729,10 +710,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1">
         <v>45334</v>
@@ -743,14 +724,14 @@
       <c r="G4">
         <v>0</v>
       </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
       <c r="I4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -761,7 +742,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1">
         <v>45334</v>
@@ -772,14 +753,14 @@
       <c r="G5">
         <v>0</v>
       </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
       <c r="I5" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -802,16 +783,13 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -819,10 +797,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
       </c>
       <c r="E7" s="1">
         <v>45335</v>
@@ -833,25 +811,22 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="I7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E8" s="1">
         <v>45344</v>
@@ -862,25 +837,25 @@
       <c r="G8">
         <v>0</v>
       </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
       <c r="I8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1">
         <v>45344</v>
@@ -891,25 +866,25 @@
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
       <c r="I9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1">
         <v>45344</v>
@@ -920,22 +895,22 @@
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="J10" t="s">
+      <c r="I10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1">
         <v>45344</v>
@@ -946,25 +921,25 @@
       <c r="G11">
         <v>0</v>
       </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
       <c r="I11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E12" s="1">
         <v>45344</v>
@@ -975,22 +950,22 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="J12" t="s">
+      <c r="I12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1">
         <v>45344</v>
@@ -1001,22 +976,22 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="J13" t="s">
+      <c r="I13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E14" s="1">
         <v>45346</v>
@@ -1027,25 +1002,25 @@
       <c r="G14">
         <v>0</v>
       </c>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
       <c r="I14" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E15" s="1">
         <v>45346</v>
@@ -1053,14 +1028,14 @@
       <c r="F15" s="1">
         <v>45388</v>
       </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
       <c r="I15" t="s">
-        <v>70</v>
-      </c>
-      <c r="J15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1068,10 +1043,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1">
         <v>45354</v>
@@ -1082,25 +1057,25 @@
       <c r="G16">
         <v>0</v>
       </c>
+      <c r="H16" t="s">
+        <v>31</v>
+      </c>
       <c r="I16" t="s">
-        <v>36</v>
-      </c>
-      <c r="J16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E17" s="1">
         <v>45336</v>
@@ -1108,22 +1083,22 @@
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="J17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E18" s="1">
         <v>45336</v>
@@ -1131,25 +1106,25 @@
       <c r="G18">
         <v>1</v>
       </c>
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
       <c r="I18" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E19" s="1">
         <v>45336</v>
@@ -1157,14 +1132,14 @@
       <c r="G19">
         <v>1</v>
       </c>
+      <c r="H19" t="s">
+        <v>54</v>
+      </c>
       <c r="I19" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1172,10 +1147,10 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E20" s="1">
         <v>45336</v>
@@ -1183,25 +1158,25 @@
       <c r="G20">
         <v>1</v>
       </c>
+      <c r="H20" t="s">
+        <v>56</v>
+      </c>
       <c r="I20" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1">
         <v>45336</v>
@@ -1209,22 +1184,22 @@
       <c r="G21">
         <v>0</v>
       </c>
-      <c r="J21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E22" s="1">
         <v>45336</v>
@@ -1232,56 +1207,56 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="J22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>